<commit_message>
adding tags to a sheet that did not annotate
</commit_message>
<xml_diff>
--- a/frack/data/operation_conakry.xlsx
+++ b/frack/data/operation_conakry.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="463" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="463" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Communication" sheetId="1" state="visible" r:id="rId2"/>
@@ -1402,22 +1402,22 @@
     <t>En cours depuis 14 Avril</t>
   </si>
   <si>
-    <t>Etablir un comité de recherche et un protocole pour toutes les études</t>
-  </si>
-  <si>
-    <t>Etablir un comité d'éthique</t>
-  </si>
-  <si>
-    <t>Etablir un conseil de sécurité pour les médicaments et vaccins et aussi un processus formel d'approbation et de suivi</t>
-  </si>
-  <si>
-    <t>Evaluation de l'impact de l'ebola sur la prise en charge du paludisme</t>
-  </si>
-  <si>
-    <t>Evaluation de l'impact de l'ebola sur les services de sante de routine (SMNI)</t>
-  </si>
-  <si>
-    <t>Donner appui technique pour faire de la recherche operationnel (mise en oeuvre) sur les nouveaux diagnostiques, traitements, et vaccins</t>
+    <t>[A]Etablir un comité de recherche et un protocole pour toutes les études</t>
+  </si>
+  <si>
+    <t>[A]Etablir un comité d'éthique</t>
+  </si>
+  <si>
+    <t>[A]Etablir un conseil de sécurité pour les médicaments et vaccins et aussi un processus formel d'approbation et de suivi</t>
+  </si>
+  <si>
+    <t>[A]Evaluation de l'impact de l'ebola sur la prise en charge du paludisme</t>
+  </si>
+  <si>
+    <t>[A]Evaluation de l'impact de l'ebola sur les services de sante de routine (SMNI)</t>
+  </si>
+  <si>
+    <t>[A]Donner appui technique pour faire de la recherche operationnel (mise en oeuvre) sur les nouveaux diagnostiques, traitements, et vaccins</t>
   </si>
   <si>
     <t>MSF; OMS</t>
@@ -2175,7 +2175,7 @@
   </sheetPr>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -5468,22 +5468,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>434</v>
@@ -5563,6 +5565,10 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5746,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
@@ -8918,10 +8924,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="59" t="s">
         <v>255</v>
@@ -8960,7 +8968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
@@ -9778,7 +9786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
@@ -11326,7 +11334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
@@ -12227,7 +12235,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="83" t="s">
         <v>342</v>
@@ -12260,7 +12268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
@@ -12325,7 +12333,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="88"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
         <v>31</v>
       </c>

</xml_diff>